<commit_message>
Actualiza población censada total
</commit_message>
<xml_diff>
--- a/Data/Tabla auxiliar proyecciones.xlsx
+++ b/Data/Tabla auxiliar proyecciones.xlsx
@@ -1,33 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\1. Unidad de Métodos y Acceso a Datos\1. Observatorio UMAD\PISO III_INDICADORES\2021\Piso_1_Demografia\Piso-I_Demografia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shari\Dropbox\UMAD\Sociodemografico\GITHUB DEFINITIVOS\Piso-I-Demografia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58A6B6E-5594-4668-B485-7F469CDFE581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="80" yWindow="180" windowWidth="19120" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t xml:space="preserve">Proy (NNUU 2019) </t>
   </si>
@@ -47,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +101,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -366,16 +378,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -386,7 +401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -397,7 +412,7 @@
         <v>2595.5100000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -408,7 +423,7 @@
         <v>2788.4290000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -419,7 +434,7 @@
         <v>2955.241</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -430,7 +445,7 @@
         <v>3163.7629999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -441,87 +456,109 @@
         <v>3286.3139999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
+        <v>2023</v>
+      </c>
+      <c r="C7">
+        <v>3444.2629999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
         <v>1950</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>2239</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
         <v>1960</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>2539</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>1970</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2810</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
         <v>1980</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>2915</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
         <v>1990</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>3110</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
         <v>2000</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>3320</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
         <v>2010</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>3359</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>2020</v>
+      </c>
+      <c r="C15">
+        <v>3473.7269999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:C13">
-    <sortCondition ref="A2:A13"/>
-    <sortCondition ref="B2:B13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
+    <sortCondition ref="A2:A14"/>
+    <sortCondition ref="B2:B14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Elimina dato 2023 de población censada
</commit_message>
<xml_diff>
--- a/Data/Tabla auxiliar proyecciones.xlsx
+++ b/Data/Tabla auxiliar proyecciones.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shari\Dropbox\UMAD\Sociodemografico\GITHUB DEFINITIVOS\Piso-I-Demografia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharo\Dropbox\UMAD\Sociodemografico\GITHUB DEFINITIVOS\Piso-I-Demografia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58A6B6E-5594-4668-B485-7F469CDFE581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4C06EB-9D98-4D74-9406-8A7CFFCA9054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="180" windowWidth="19120" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
   <si>
     <t xml:space="preserve">Proy (NNUU 2019) </t>
   </si>
@@ -379,18 +379,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -401,7 +401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -412,7 +412,7 @@
         <v>2595.5100000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -423,7 +423,7 @@
         <v>2788.4290000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -434,7 +434,7 @@
         <v>2955.241</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -445,7 +445,7 @@
         <v>3163.7629999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -456,109 +456,98 @@
         <v>3286.3139999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>2023</v>
+        <v>1950</v>
       </c>
       <c r="C7">
-        <v>3444.2629999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8">
-        <v>1950</v>
+        <v>1960</v>
       </c>
       <c r="C8">
-        <v>2239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
-        <v>1960</v>
+        <v>1970</v>
       </c>
       <c r="C9">
-        <v>2539</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10">
-        <v>1970</v>
+        <v>1980</v>
       </c>
       <c r="C10">
-        <v>2810</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1980</v>
+        <v>1990</v>
       </c>
       <c r="C11">
-        <v>2915</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="C12">
-        <v>3110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="C13">
-        <v>3320</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="C14">
-        <v>3359</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>2020</v>
-      </c>
-      <c r="C15">
         <v>3473.7269999999999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
-    <sortCondition ref="A2:A14"/>
-    <sortCondition ref="B2:B14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C13">
+    <sortCondition ref="A2:A13"/>
+    <sortCondition ref="B2:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>